<commit_message>
Basic fixes to docs
</commit_message>
<xml_diff>
--- a/data-raw/saros_function_names.xlsx
+++ b/data-raw/saros_function_names.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nifu-my.sharepoint.com/personal/stephan_daus_nifu_no/Documents/Github-R/surveyreport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nifu-my.sharepoint.com/personal/stephan_daus_nifu_no/Documents/Github-R/saros/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{B3C19227-06CD-469E-AA97-648992118E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{522A51C5-A543-4E3C-9E20-3DE74AA3BEA5}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{B3C19227-06CD-469E-AA97-648992118E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FFF2443-B23A-46C8-BD1E-F1EEAABFEE05}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0B6B4A4A-2D40-4A92-8233-3D0C6721FB0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="surveyreport Functions" sheetId="1" r:id="rId1"/>
-    <sheet name="text" sheetId="2" r:id="rId2"/>
+    <sheet name="text" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,28 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
-  <si>
-    <t>Extract from (3)</t>
-  </si>
-  <si>
-    <t>loop_sigtest(by=NULL)</t>
-  </si>
-  <si>
-    <t>Significance testing</t>
-  </si>
-  <si>
-    <t>Extract by battery ID from (3) and add table/graph number</t>
-  </si>
-  <si>
-    <t>describe_univariates</t>
-  </si>
-  <si>
-    <t>4. Embed in document</t>
-  </si>
-  <si>
-    <t>3. Loop (2) across all batteries</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Kvinne</t>
   </si>
@@ -135,42 +113,6 @@
     <t>Snitt</t>
   </si>
   <si>
-    <t>Map of PSUs for HTML/PDF</t>
-  </si>
-  <si>
-    <t>Map of PSUs for Word</t>
-  </si>
-  <si>
-    <t>packages</t>
-  </si>
-  <si>
-    <t>mschart</t>
-  </si>
-  <si>
-    <t>ggiraph</t>
-  </si>
-  <si>
-    <t>reactable</t>
-  </si>
-  <si>
-    <t>crosstable/flextable/officer</t>
-  </si>
-  <si>
-    <t>officer</t>
-  </si>
-  <si>
-    <t>ggiraph, sf</t>
-  </si>
-  <si>
-    <t>ggplot2</t>
-  </si>
-  <si>
-    <t>infer</t>
-  </si>
-  <si>
-    <t>map_psus</t>
-  </si>
-  <si>
     <t>intro</t>
   </si>
   <si>
@@ -199,127 +141,13 @@
   </si>
   <si>
     <t>mean_diff</t>
-  </si>
-  <si>
-    <t>summarize_data(by=NULL)</t>
-  </si>
-  <si>
-    <t>summarize_data_sigtest(by=NULL)</t>
-  </si>
-  <si>
-    <t>1. Prepare dataset</t>
-  </si>
-  <si>
-    <t>chart_categorical_office</t>
-  </si>
-  <si>
-    <t>text_categorical_interactive</t>
-  </si>
-  <si>
-    <t>text_categorical_office</t>
-  </si>
-  <si>
-    <t>Likert plot for Office</t>
-  </si>
-  <si>
-    <t>Crosstable for Office</t>
-  </si>
-  <si>
-    <t>Descriptives text for Office</t>
-  </si>
-  <si>
-    <t>Likert plot for HTML</t>
-  </si>
-  <si>
-    <t>Crosstable for HTML</t>
-  </si>
-  <si>
-    <t>Descriptives text for HTML</t>
-  </si>
-  <si>
-    <t>loop_interactive_chart_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>loop_static_chart_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>loop_interactive_table_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>loop_static_table_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>loop_interactive_text_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>loop_static_text_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>2. Create base element (hidden)</t>
-  </si>
-  <si>
-    <t>3. Checks, call summary_data and create base element</t>
-  </si>
-  <si>
-    <t>chart_interactive_chart_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>chart_static_chart_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>chart_static_table_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>chart_interactive_text_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>chart_static_text_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>chart_sigtest(by=NULL)</t>
-  </si>
-  <si>
-    <t>chart_categorical_interactive</t>
-  </si>
-  <si>
-    <t>embed_tabulate_interactive_table_categorical(by=NULL)</t>
-  </si>
-  <si>
-    <t>table_categorical_office</t>
-  </si>
-  <si>
-    <t>table_categorical_interactive</t>
-  </si>
-  <si>
-    <t>test_categorical</t>
-  </si>
-  <si>
-    <t>interactive_categorical_chart</t>
-  </si>
-  <si>
-    <t>interactive_categorical_table</t>
-  </si>
-  <si>
-    <t>interactive_categorical_text</t>
-  </si>
-  <si>
-    <t>static_categorical_chart</t>
-  </si>
-  <si>
-    <t>static_categorical_table</t>
-  </si>
-  <si>
-    <t>static_categorical_text</t>
-  </si>
-  <si>
-    <t>sigtest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,23 +157,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -373,17 +184,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,9 +205,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -442,7 +245,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -548,7 +351,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -690,289 +493,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38428D25-4E0C-40B9-BE21-8463260EA876}">
-  <dimension ref="A1:G24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.88671875" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
-    <col min="6" max="6" width="38.33203125" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="D16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="D17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7FE9AA-784E-40AF-A764-D7436FDA7C22}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -984,33 +515,33 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -1036,15 +567,15 @@
         <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1070,15 +601,15 @@
         <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -1104,15 +635,15 @@
         <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>60</v>
@@ -1138,15 +669,15 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -1172,66 +703,66 @@
         <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J7" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J8" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -1249,7 +780,7 @@
         <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1257,7 +788,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -1277,10 +808,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -1303,7 +834,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -1323,10 +854,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>40</v>
@@ -1349,7 +880,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1369,10 +900,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>60</v>
@@ -1395,7 +926,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>0</v>

</xml_diff>